<commit_message>
Remove node_modules from repo, update gitignore
</commit_message>
<xml_diff>
--- a/Redmine_org_Test_Cases.xlsx
+++ b/Redmine_org_Test_Cases.xlsx
@@ -721,8 +721,8 @@
   </sheetPr>
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28125" defaultRowHeight="74.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
change name for test (to avoid misunderstandings about API testing)
</commit_message>
<xml_diff>
--- a/Redmine_org_Test_Cases.xlsx
+++ b/Redmine_org_Test_Cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="116">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -28,10 +28,10 @@
     <t xml:space="preserve">Title</t>
   </si>
   <si>
-    <t xml:space="preserve">API‑001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify REST API documentation page and method blocks</t>
+    <t xml:space="preserve">UI_DOC_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify presence of REST API documentation on the website</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -60,6 +60,9 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">*Note: This is not an API test. It only verifies UI navigation to the documentation page.*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Click 'Developer's Guide' link</t>
   </si>
   <si>
@@ -108,7 +111,7 @@
     <t xml:space="preserve">Clicking the ‘Updating a project' link scrolls to the correct section</t>
   </si>
   <si>
-    <t xml:space="preserve">API‑002</t>
+    <t xml:space="preserve">UI_DOC_002</t>
   </si>
   <si>
     <t xml:space="preserve">Check navigation of breadcrumbs</t>
@@ -151,7 +154,7 @@
     <t xml:space="preserve">AUTH-001</t>
   </si>
   <si>
-    <t xml:space="preserve">Check Sing In with invalid data  and check ‘Lost Password’ with invalid data</t>
+    <t xml:space="preserve">Check Sign In with invalid data  and check ‘Lost Password’ with invalid data</t>
   </si>
   <si>
     <t xml:space="preserve">Opened Home page as non-registered user.</t>
@@ -298,7 +301,7 @@
     <t xml:space="preserve">Field contains value ‘is’</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that the dropdown list of statuses displayed</t>
+    <t xml:space="preserve">Verify that the dropdown list of operators is visible</t>
   </si>
   <si>
     <t xml:space="preserve">Dropdown list of statuses displayed</t>
@@ -313,7 +316,10 @@
     <t xml:space="preserve">Click outside the field to apply the filter</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that all listed issues on the 1 page have the {test status}  status</t>
+    <t xml:space="preserve">The filter is applied and results are reloaded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All listed issues have the status {test status}</t>
   </si>
   <si>
     <t xml:space="preserve">Only issues with {test status}  status are shown</t>
@@ -334,7 +340,7 @@
     <t xml:space="preserve">DL-001</t>
   </si>
   <si>
-    <t xml:space="preserve">Check download of the latest Release</t>
+    <t xml:space="preserve">Verify latest release archive is listed and downloadable</t>
   </si>
   <si>
     <t xml:space="preserve">Opened Download page (/projects/redmine/wiki/Download)</t>
@@ -349,7 +355,7 @@
     <t xml:space="preserve">Latest releases' section is visible</t>
   </si>
   <si>
-    <t xml:space="preserve">Check the table contains {latest release}</t>
+    <t xml:space="preserve">Verify that the table includes an entry for {latest release}</t>
   </si>
   <si>
     <t xml:space="preserve">{latest release} is present and visible</t>
@@ -364,7 +370,7 @@
     <t xml:space="preserve">Click the '{latest release}.zip' link</t>
   </si>
   <si>
-    <t xml:space="preserve">The '.zip' link starts downloading the archive</t>
+    <t xml:space="preserve">File download is triggered with '{latest release}.zip' file name</t>
   </si>
 </sst>
 </file>
@@ -379,6 +385,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -400,17 +407,20 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -467,72 +477,88 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,8 +747,8 @@
   </sheetPr>
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C85" activeCellId="0" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28125" defaultRowHeight="74.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,57 +761,57 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" s="7" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -793,157 +819,163 @@
       <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>11</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="0"/>
+      <c r="C9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="45.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="0"/>
+      <c r="C10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="37.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="0"/>
+      <c r="C11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="0"/>
+      <c r="C12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="C13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" s="3" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" s="4" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" s="7" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="B16" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" s="9" customFormat="true" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="n">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" s="11" customFormat="true" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="B18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" s="13" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -951,692 +983,695 @@
       <c r="A20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="B20" s="14" t="s">
         <v>32</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="29.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="14" t="s">
         <v>34</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="26.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>35</v>
+      <c r="B22" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="B23" s="14" t="s">
         <v>37</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="B24" s="14" t="s">
         <v>39</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>35</v>
+      <c r="B25" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" s="3" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" s="4" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" s="7" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="B28" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="n">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="6" t="s">
+      <c r="B30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" s="13" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="B32" s="17" t="s">
         <v>45</v>
       </c>
+      <c r="C32" s="17" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="31.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="B33" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="C33" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="B34" s="17" t="s">
         <v>49</v>
       </c>
+      <c r="C34" s="17" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="32.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="0" t="s">
+      <c r="A35" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>51</v>
       </c>
+      <c r="C35" s="17" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="0" t="s">
+      <c r="B36" s="17" t="s">
         <v>53</v>
       </c>
+      <c r="C36" s="17" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="33.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="0" t="s">
+      <c r="B37" s="17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" s="3" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C37" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="13" t="s">
+      <c r="A39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" s="7" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="B39" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+    </row>
+    <row r="40" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="n">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="n">
+      <c r="B41" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-    </row>
-    <row r="43" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="16" t="s">
+      <c r="B42" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-    </row>
-    <row r="44" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8"/>
-      <c r="B44" s="14" t="s">
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+    </row>
+    <row r="43" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-    </row>
-    <row r="45" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10"/>
+      <c r="B44" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+    </row>
+    <row r="45" s="13" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="0" t="s">
+      <c r="B46" s="17" t="s">
         <v>63</v>
       </c>
+      <c r="C46" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="0" t="s">
+      <c r="B47" s="17" t="s">
         <v>65</v>
       </c>
+      <c r="C47" s="17" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="24.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="0" t="s">
+      <c r="B48" s="17" t="s">
         <v>67</v>
       </c>
+      <c r="C48" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" s="0" t="s">
+      <c r="A49" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>69</v>
       </c>
+      <c r="C49" s="17" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="21.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B50" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="0" t="s">
+      <c r="B50" s="17" t="s">
         <v>71</v>
       </c>
+      <c r="C50" s="17" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="21.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="0" t="s">
+      <c r="B51" s="17" t="s">
         <v>73</v>
       </c>
+      <c r="C51" s="17" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="0" t="s">
+      <c r="B52" s="17" t="s">
         <v>75</v>
       </c>
+      <c r="C52" s="17" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="21.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="0" t="s">
+      <c r="B53" s="17" t="s">
         <v>77</v>
       </c>
+      <c r="C53" s="17" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="0" t="s">
+      <c r="B54" s="17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="55" s="3" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C54" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" s="4" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="13" t="s">
+      <c r="A56" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-    </row>
-    <row r="57" s="7" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="6" t="s">
+      <c r="B56" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+    </row>
+    <row r="57" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8" t="n">
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-    </row>
-    <row r="59" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="n">
+      <c r="B58" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B59" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-    </row>
-    <row r="60" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-    </row>
-    <row r="61" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8"/>
-      <c r="B61" s="14" t="s">
+      <c r="B59" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-    </row>
-    <row r="62" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="6" t="s">
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+    </row>
+    <row r="60" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+    </row>
+    <row r="61" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10"/>
+      <c r="B61" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+    </row>
+    <row r="62" s="13" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="28.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B63" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="0" t="s">
+      <c r="B63" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="0"/>
+      <c r="C63" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B64" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="0" t="s">
+      <c r="B64" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D64" s="0"/>
+      <c r="C64" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="0" t="s">
+      <c r="B65" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="0"/>
+      <c r="C65" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" s="17"/>
     </row>
     <row r="66" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" s="0" t="s">
+      <c r="A66" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="0"/>
+      <c r="C66" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C67" s="0" t="s">
+      <c r="B67" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D67" s="0"/>
+      <c r="C67" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D67" s="17"/>
     </row>
     <row r="68" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+      <c r="A68" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B68" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="0"/>
-      <c r="D68" s="0"/>
+      <c r="B68" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="17"/>
     </row>
     <row r="69" customFormat="false" ht="31.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D69" s="0"/>
+      <c r="B69" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="17"/>
     </row>
     <row r="70" customFormat="false" ht="31.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+      <c r="A70" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="B70" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D70" s="0"/>
+      <c r="B70" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70" s="17"/>
     </row>
     <row r="71" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="B71" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D71" s="0"/>
-    </row>
-    <row r="72" s="3" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D71" s="17"/>
+    </row>
+    <row r="72" s="4" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-    </row>
-    <row r="74" s="7" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" s="6" t="s">
+      <c r="A73" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+    </row>
+    <row r="74" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-    </row>
-    <row r="75" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8" t="n">
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
-    </row>
-    <row r="77" s="9" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8"/>
-      <c r="B77" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-    </row>
-    <row r="78" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78" s="6" t="s">
+      <c r="B75" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+    </row>
+    <row r="77" s="11" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="10"/>
+      <c r="B77" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+    </row>
+    <row r="78" s="13" customFormat="true" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D78" s="10" t="s">
+      <c r="D78" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+      <c r="A79" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>107</v>
+      <c r="B79" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
+      <c r="A80" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B80" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>109</v>
+      <c r="B80" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
+      <c r="A81" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B81" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>111</v>
+      <c r="B81" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>113</v>
+      <c r="A82" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0"/>
-      <c r="B83" s="0"/>
-      <c r="C83" s="0"/>
+      <c r="A83" s="17"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
     </row>
     <row r="84" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="0"/>
+      <c r="C84" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="D6:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>

</xml_diff>